<commit_message>
in import data employee add email office,  add role able action import (SA, Admin, Admin HR), and remove example data
</commit_message>
<xml_diff>
--- a/public/assets/file/template/Import_Employee_Data_MSK.xlsx
+++ b/public/assets/file/template/Import_Employee_Data_MSK.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project Code\Laravel 10\recruitment_be_msk\public\assets\file\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64572678-30A2-4D8B-A8D7-DE2E539CC7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DFA78CD-A69F-4A37-94B8-2AD402E07211}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{58682AD7-F932-443F-B577-CFB4A383E950}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
-  <si>
-    <t>Email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>NIK</t>
   </si>
@@ -56,27 +53,12 @@
     <t>Nama Depan</t>
   </si>
   <si>
-    <t>Nama Belakang</t>
-  </si>
-  <si>
-    <t>Jenis Kelamin</t>
-  </si>
-  <si>
     <t>Tempat Lahir</t>
   </si>
   <si>
-    <t>Tanggal Lahir</t>
-  </si>
-  <si>
-    <t>Status Pernikahan</t>
-  </si>
-  <si>
     <t>No. HP</t>
   </si>
   <si>
-    <t>Tanggal Bergabung</t>
-  </si>
-  <si>
     <t>Divisi</t>
   </si>
   <si>
@@ -92,88 +74,47 @@
     <t>Email Reportline 1</t>
   </si>
   <si>
-    <t>Email Reportline 5</t>
-  </si>
-  <si>
-    <t>Email Reportline 4</t>
-  </si>
-  <si>
     <t>Email Reportline 3</t>
   </si>
   <si>
     <t>Email Reportline 2</t>
   </si>
   <si>
-    <t>Male/Female</t>
-  </si>
-  <si>
-    <t>Jakarta Selatan</t>
-  </si>
-  <si>
-    <t>Single/Married/Divorce</t>
-  </si>
-  <si>
-    <t>example@xyz.com</t>
-  </si>
-  <si>
-    <t>Jalan Raya Pandeglang KM. 3, Karundang, Cipocok Jaya, Kota Serang, Banten, 42125</t>
-  </si>
-  <si>
-    <t>Operational</t>
-  </si>
-  <si>
-    <t>Marketing</t>
-  </si>
-  <si>
-    <t>Area Sales Officer</t>
-  </si>
-  <si>
-    <t>Mitra Sendang Kemakmuran</t>
-  </si>
-  <si>
-    <t>example1@xyz.com</t>
-  </si>
-  <si>
-    <t>example2@xyz.com</t>
-  </si>
-  <si>
-    <t>example3@xyz.com</t>
-  </si>
-  <si>
-    <t>opsional</t>
-  </si>
-  <si>
-    <t>081234567890</t>
-  </si>
-  <si>
-    <t>Jangan Hapus</t>
-  </si>
-  <si>
-    <t>Contoh Isian</t>
+    <t>Jenis Kelamin (Male/Female)</t>
+  </si>
+  <si>
+    <t>Status Pernikahan (Single/Married/Divorce)</t>
+  </si>
+  <si>
+    <t>Tanggal Bergabung (1/1/2016)</t>
+  </si>
+  <si>
+    <t>Tanggal Lahir (1/1/1990)</t>
+  </si>
+  <si>
+    <t>Email Reportline 4 (Opsional)</t>
+  </si>
+  <si>
+    <t>Email Reportline 5 (Opsional)</t>
+  </si>
+  <si>
+    <t>Nama Belakang (Opsional)</t>
+  </si>
+  <si>
+    <t>Email Pribadi</t>
+  </si>
+  <si>
+    <t>Email Kantor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -187,7 +128,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -197,12 +138,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -231,23 +166,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -580,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA42B7CA-F844-4C18-87EC-841289318263}">
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:W1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -591,165 +519,96 @@
     <col min="1" max="1" width="16.453125" customWidth="1"/>
     <col min="2" max="2" width="15.453125" customWidth="1"/>
     <col min="3" max="3" width="18.36328125" customWidth="1"/>
-    <col min="4" max="4" width="19.7265625" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-    <col min="6" max="6" width="14.453125" customWidth="1"/>
-    <col min="7" max="7" width="15" customWidth="1"/>
-    <col min="8" max="8" width="22.6328125" customWidth="1"/>
-    <col min="9" max="9" width="18.26953125" customWidth="1"/>
-    <col min="10" max="10" width="15.54296875" style="8" customWidth="1"/>
-    <col min="11" max="12" width="68.7265625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.90625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.26953125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23.54296875" bestFit="1" customWidth="1"/>
-    <col min="18" max="22" width="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" customWidth="1"/>
+    <col min="5" max="5" width="27.453125" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
+    <col min="7" max="7" width="24.54296875" customWidth="1"/>
+    <col min="8" max="8" width="37.7265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23.7265625" customWidth="1"/>
+    <col min="10" max="10" width="24.08984375" customWidth="1"/>
+    <col min="11" max="11" width="15.54296875" style="3" customWidth="1"/>
+    <col min="12" max="13" width="68.7265625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.81640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1796875" customWidth="1"/>
+    <col min="16" max="16" width="14.36328125" customWidth="1"/>
+    <col min="17" max="17" width="16.453125" customWidth="1"/>
+    <col min="18" max="18" width="26.7265625" customWidth="1"/>
+    <col min="19" max="21" width="17" bestFit="1" customWidth="1"/>
+    <col min="22" max="23" width="25.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="S1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="M1" s="1" t="s">
+      <c r="T1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>123</v>
-      </c>
-      <c r="B2" s="2">
-        <v>123</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="3">
-        <v>32874</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="J2" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" s="3">
-        <v>42005</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>34</v>
+      <c r="W1" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{1EAEB3CE-49A6-49D9-BB6B-13593134B075}"/>
-    <hyperlink ref="R2" r:id="rId2" xr:uid="{2580E210-F84F-4334-8109-B0DA10EFA460}"/>
-    <hyperlink ref="S2" r:id="rId3" xr:uid="{0013BFC1-7D94-483F-B24F-7462B92B8114}"/>
-    <hyperlink ref="T2" r:id="rId4" xr:uid="{236D0668-18FA-4FF4-8586-86627DEE76B5}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>